<commit_message>
Use updated export files
</commit_message>
<xml_diff>
--- a/data/export/country.xlsx
+++ b/data/export/country.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="851" count="851">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="987" count="987">
   <x:si>
     <x:t>ISO3</x:t>
   </x:si>
@@ -1423,16 +1423,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>5440619</x:v>
+        <x:v>6440206</x:v>
       </x:c>
       <x:c r="I3" s="0" t="n">
-        <x:v>52099172.5</x:v>
+        <x:v>57134693.33</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:9">
@@ -1501,16 +1501,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>2572547</x:v>
+        <x:v>5531997</x:v>
       </x:c>
       <x:c r="I6" s="0" t="n">
-        <x:v>9616032</x:v>
+        <x:v>43333075.9</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:9">
@@ -1533,13 +1533,13 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="G7" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
         <x:v>8347448.43</x:v>
       </x:c>
       <x:c r="I7" s="0" t="n">
-        <x:v>39373195</x:v>
+        <x:v>53941307.47</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:9">
@@ -1568,7 +1568,7 @@
         <x:v>6198092</x:v>
       </x:c>
       <x:c r="I8" s="0" t="n">
-        <x:v>225408286.31</x:v>
+        <x:v>228791472.01</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:9">
@@ -1588,16 +1588,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F9" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G9" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="H9" s="0" t="n">
-        <x:v>5206305.39</x:v>
+        <x:v>5934761.39</x:v>
       </x:c>
       <x:c r="I9" s="0" t="n">
-        <x:v>157028123.07</x:v>
+        <x:v>195140680.35</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9">
@@ -1617,16 +1617,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>3841560</x:v>
+        <x:v>4672380</x:v>
       </x:c>
       <x:c r="I10" s="0" t="n">
-        <x:v>46493937.3</x:v>
+        <x:v>73993937.3</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:9">
@@ -1646,13 +1646,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>5599696.35</x:v>
+        <x:v>8599693.35</x:v>
       </x:c>
       <x:c r="I11" s="0" t="n">
         <x:v>44266339.28</x:v>
@@ -1704,13 +1704,13 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
         <x:v>6120068.78</x:v>
       </x:c>
       <x:c r="I13" s="0" t="n">
-        <x:v>441165030</x:v>
+        <x:v>464313178.15</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:9">
@@ -1733,13 +1733,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>1516737</x:v>
+        <x:v>1217354</x:v>
       </x:c>
       <x:c r="I14" s="0" t="n">
-        <x:v>236984296.53</x:v>
+        <x:v>245272547.98</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:9">
@@ -1759,16 +1759,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>9043326.6</x:v>
+        <x:v>10043311.6</x:v>
       </x:c>
       <x:c r="I15" s="0" t="n">
-        <x:v>47707835.32</x:v>
+        <x:v>66450633.07</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:9">
@@ -1788,16 +1788,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>4838662.39</x:v>
+        <x:v>7114158.39</x:v>
       </x:c>
       <x:c r="I16" s="0" t="n">
-        <x:v>87358124.14</x:v>
+        <x:v>94903883</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:9">
@@ -1817,13 +1817,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>6362286</x:v>
+        <x:v>7262254.44</x:v>
       </x:c>
       <x:c r="I17" s="0" t="n">
         <x:v>61904548</x:v>
@@ -1846,16 +1846,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>2627919.74</x:v>
+        <x:v>6627842.9</x:v>
       </x:c>
       <x:c r="I18" s="0" t="n">
-        <x:v>33300000</x:v>
+        <x:v>102186669.84</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:9">
@@ -1875,13 +1875,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F19" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="G19" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="H19" s="0" t="n">
-        <x:v>3703756</x:v>
+        <x:v>4702738</x:v>
       </x:c>
       <x:c r="I19" s="0" t="n">
         <x:v>31746000</x:v>
@@ -1933,16 +1933,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>5164666.81</x:v>
+        <x:v>8362518.81</x:v>
       </x:c>
       <x:c r="I21" s="0" t="n">
-        <x:v>443700100.86</x:v>
+        <x:v>671916084.37</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:9">
@@ -1985,16 +1985,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>5303415</x:v>
+        <x:v>5988156</x:v>
       </x:c>
       <x:c r="I23" s="0" t="n">
-        <x:v>144777909.2</x:v>
+        <x:v>206140643.33</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:9">
@@ -2043,13 +2043,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>1996311</x:v>
+        <x:v>5793747</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:9">
@@ -2072,13 +2072,13 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
         <x:v>5633291.76</x:v>
       </x:c>
       <x:c r="I26" s="0" t="n">
-        <x:v>240097216</x:v>
+        <x:v>357454221.66</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:9">
@@ -2101,13 +2101,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
         <x:v>3768098</x:v>
       </x:c>
       <x:c r="I27" s="0" t="n">
-        <x:v>60458971.14</x:v>
+        <x:v>81957000.5</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:9">
@@ -2127,13 +2127,13 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>1771129</x:v>
+        <x:v>2770944</x:v>
       </x:c>
       <x:c r="I28" s="0" t="n">
         <x:v>39998000</x:v>
@@ -2156,16 +2156,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>3587979</x:v>
+        <x:v>5405215</x:v>
       </x:c>
       <x:c r="I29" s="0" t="n">
-        <x:v>78286169.72</x:v>
+        <x:v>103844297.82</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:9">
@@ -2185,13 +2185,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>7</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>7261503.86</x:v>
+        <x:v>8118061.86</x:v>
       </x:c>
       <x:c r="I30" s="0" t="n">
         <x:v>175518677</x:v>
@@ -2243,13 +2243,13 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
         <x:v>7128093.27</x:v>
       </x:c>
       <x:c r="I32" s="0" t="n">
-        <x:v>315101202.64</x:v>
+        <x:v>364598817.91</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:9">
@@ -2269,13 +2269,13 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>2121256</x:v>
+        <x:v>5099665</x:v>
       </x:c>
       <x:c r="I33" s="0" t="n">
         <x:v>66724236.16</x:v>
@@ -2298,13 +2298,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>1266397</x:v>
+        <x:v>2265781.06</x:v>
       </x:c>
       <x:c r="I34" s="0" t="n">
         <x:v>28988852</x:v>
@@ -2330,13 +2330,13 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
         <x:v>8565348.47</x:v>
       </x:c>
       <x:c r="I35" s="0" t="n">
-        <x:v>24421593.8</x:v>
+        <x:v>71925448.92</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:9">
@@ -2359,13 +2359,13 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>5955062.29</x:v>
+        <x:v>6599988.84</x:v>
       </x:c>
       <x:c r="I36" s="0" t="n">
-        <x:v>410948911.6</x:v>
+        <x:v>423497027.85</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:9">
@@ -2385,16 +2385,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>6349045</x:v>
+        <x:v>7274838</x:v>
       </x:c>
       <x:c r="I37" s="0" t="n">
-        <x:v>145572752.53</x:v>
+        <x:v>184102430.51</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:9">
@@ -2414,13 +2414,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>6457324.16</x:v>
+        <x:v>6957236.16</x:v>
       </x:c>
       <x:c r="I38" s="0" t="n">
         <x:v>62134085</x:v>
@@ -2478,7 +2478,7 @@
         <x:v>3688739</x:v>
       </x:c>
       <x:c r="I40" s="0" t="n">
-        <x:v>113138919.15</x:v>
+        <x:v>114501329.75</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:9">
@@ -2498,16 +2498,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>1606325.13</x:v>
+        <x:v>4387798.04</x:v>
       </x:c>
       <x:c r="I41" s="0" t="n">
-        <x:v>67349239.38</x:v>
+        <x:v>75017226.8</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:9">
@@ -2527,16 +2527,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>7240872.42</x:v>
+        <x:v>7300759.42</x:v>
       </x:c>
       <x:c r="I42" s="0" t="n">
-        <x:v>26678585</x:v>
+        <x:v>51205254</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:9">
@@ -2562,10 +2562,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>5774918.99</x:v>
+        <x:v>7624887.99</x:v>
       </x:c>
       <x:c r="I43" s="0" t="n">
-        <x:v>103309571.84</x:v>
+        <x:v>104798949.68</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:9">
@@ -2585,16 +2585,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>8324247.38</x:v>
+        <x:v>9324246.36</x:v>
       </x:c>
       <x:c r="I44" s="0" t="n">
-        <x:v>297727896.34</x:v>
+        <x:v>337114797.79</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:9">
@@ -2617,13 +2617,13 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
         <x:v>4188953</x:v>
       </x:c>
       <x:c r="I45" s="0" t="n">
-        <x:v>338375920</x:v>
+        <x:v>369249068.15</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:9">
@@ -2643,16 +2643,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>9</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>5515044.01</x:v>
+        <x:v>6386201.01</x:v>
       </x:c>
       <x:c r="I46" s="0" t="n">
-        <x:v>112751678.4</x:v>
+        <x:v>113488173.86</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:9">
@@ -2672,13 +2672,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>2882680</x:v>
+        <x:v>5087680</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:9">
@@ -2707,7 +2707,7 @@
         <x:v>3454345</x:v>
       </x:c>
       <x:c r="I48" s="0" t="n">
-        <x:v>8366601.68</x:v>
+        <x:v>9296224.09</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:9">
@@ -2733,7 +2733,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>6833157</x:v>
+        <x:v>6534125.26</x:v>
       </x:c>
       <x:c r="I49" s="0" t="n">
         <x:v>5561000</x:v>
@@ -2759,13 +2759,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>4489895</x:v>
+        <x:v>4262617</x:v>
       </x:c>
       <x:c r="I50" s="0" t="n">
-        <x:v>371913537.57</x:v>
+        <x:v>398767876.82</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:9">
@@ -2788,13 +2788,13 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
         <x:v>3483328</x:v>
       </x:c>
       <x:c r="I51" s="0" t="n">
-        <x:v>50551985</x:v>
+        <x:v>72979078.23</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:9">
@@ -2814,16 +2814,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>2286820.7</x:v>
+        <x:v>3286820.7</x:v>
       </x:c>
       <x:c r="I52" s="0" t="n">
-        <x:v>61142559.15</x:v>
+        <x:v>58356329.25</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:9">
@@ -2852,7 +2852,7 @@
         <x:v>4088956</x:v>
       </x:c>
       <x:c r="I53" s="0" t="n">
-        <x:v>62937818.36</x:v>
+        <x:v>60151588.46</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:9">
@@ -2875,13 +2875,13 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="G54" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H54" s="0" t="n">
         <x:v>4181549.39</x:v>
       </x:c>
       <x:c r="I54" s="0" t="n">
-        <x:v>141794259.78</x:v>
+        <x:v>174208301.57</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:9">
@@ -2904,13 +2904,13 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="G55" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H55" s="0" t="n">
         <x:v>5704660</x:v>
       </x:c>
       <x:c r="I55" s="0" t="n">
-        <x:v>133201607.33</x:v>
+        <x:v>205840863.06</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:9">
@@ -2939,7 +2939,7 @@
         <x:v>4652547.43</x:v>
       </x:c>
       <x:c r="I56" s="0" t="n">
-        <x:v>59427315.63</x:v>
+        <x:v>63511817.36</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:9">
@@ -2968,7 +2968,7 @@
         <x:v>5971321.7</x:v>
       </x:c>
       <x:c r="I57" s="0" t="n">
-        <x:v>112525335.68</x:v>
+        <x:v>113067674.57</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:9">
@@ -2988,16 +2988,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F58" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G58" s="0" t="n">
         <x:v>8</x:v>
       </x:c>
       <x:c r="H58" s="0" t="n">
-        <x:v>4740117</x:v>
+        <x:v>6110117</x:v>
       </x:c>
       <x:c r="I58" s="0" t="n">
-        <x:v>73481384.16</x:v>
+        <x:v>70889310.83</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:9">
@@ -3026,7 +3026,7 @@
         <x:v>3862642</x:v>
       </x:c>
       <x:c r="I59" s="0" t="n">
-        <x:v>30954289.58</x:v>
+        <x:v>32131010.65</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:9">
@@ -3046,13 +3046,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F60" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G60" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="H60" s="0" t="n">
-        <x:v>2641041.71</x:v>
+        <x:v>3638310.71</x:v>
       </x:c>
       <x:c r="I60" s="0" t="n">
         <x:v>28637594.8</x:v>
@@ -3113,7 +3113,7 @@
         <x:v>6307987.51</x:v>
       </x:c>
       <x:c r="I62" s="0" t="n">
-        <x:v>72775066.4</x:v>
+        <x:v>73511561.86</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:9">
@@ -3136,13 +3136,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G63" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H63" s="0" t="n">
         <x:v>5600000</x:v>
       </x:c>
       <x:c r="I63" s="0" t="n">
-        <x:v>803875903.89</x:v>
+        <x:v>1048873793.89</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:9">
@@ -3165,13 +3165,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G64" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H64" s="0" t="n">
         <x:v>7555002</x:v>
       </x:c>
       <x:c r="I64" s="0" t="n">
-        <x:v>624649609.42</x:v>
+        <x:v>589275529.68</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:9">
@@ -3191,13 +3191,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F65" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="G65" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H65" s="0" t="n">
-        <x:v>1406053</x:v>
+        <x:v>4406053</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:9">
@@ -3220,13 +3220,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G66" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="H66" s="0" t="n">
         <x:v>5195033.4</x:v>
       </x:c>
       <x:c r="I66" s="0" t="n">
-        <x:v>29252000</x:v>
+        <x:v>49473682</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:9">
@@ -3272,13 +3272,13 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="G68" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H68" s="0" t="n">
-        <x:v>6599056.5</x:v>
+        <x:v>7025321</x:v>
       </x:c>
       <x:c r="I68" s="0" t="n">
-        <x:v>55879877.2</x:v>
+        <x:v>67643847</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:9">
@@ -3298,16 +3298,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F69" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="G69" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H69" s="0" t="n">
-        <x:v>4668869.4</x:v>
+        <x:v>5668827.4</x:v>
       </x:c>
       <x:c r="I69" s="0" t="n">
-        <x:v>160027625.5</x:v>
+        <x:v>456146340.78</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:9">
@@ -3330,13 +3330,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="G70" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H70" s="0" t="n">
         <x:v>4334182</x:v>
       </x:c>
       <x:c r="I70" s="0" t="n">
-        <x:v>188978785.74</x:v>
+        <x:v>216478785.74</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:9">
@@ -3356,16 +3356,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F71" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G71" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="H71" s="0" t="n">
-        <x:v>5770483</x:v>
+        <x:v>6457383</x:v>
       </x:c>
       <x:c r="I71" s="0" t="n">
-        <x:v>310345391.3</x:v>
+        <x:v>438058438.31</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:9">
@@ -3388,13 +3388,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="G72" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="H72" s="0" t="n">
         <x:v>1582874</x:v>
       </x:c>
       <x:c r="I72" s="0" t="n">
-        <x:v>28631020</x:v>
+        <x:v>36152500.12</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:9">
@@ -3437,16 +3437,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F74" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G74" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H74" s="0" t="n">
-        <x:v>4340342</x:v>
+        <x:v>5339944</x:v>
       </x:c>
       <x:c r="I74" s="0" t="n">
-        <x:v>89766913.74</x:v>
+        <x:v>117266913.74</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:9">
@@ -3466,16 +3466,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F75" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G75" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H75" s="0" t="n">
-        <x:v>8092428.75</x:v>
+        <x:v>9092428.75</x:v>
       </x:c>
       <x:c r="I75" s="0" t="n">
-        <x:v>200131967.5</x:v>
+        <x:v>267151068.83</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:9">
@@ -3495,13 +3495,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F76" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G76" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="H76" s="0" t="n">
-        <x:v>4498891.4</x:v>
+        <x:v>5498891.4</x:v>
       </x:c>
       <x:c r="I76" s="0" t="n">
         <x:v>4008985</x:v>
@@ -3556,13 +3556,13 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="G78" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="H78" s="0" t="n">
         <x:v>4438792.7</x:v>
       </x:c>
       <x:c r="I78" s="0" t="n">
-        <x:v>44469563.5</x:v>
+        <x:v>47069563.5</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:9">
@@ -3611,13 +3611,13 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="G80" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H80" s="0" t="n">
         <x:v>3061538.46</x:v>
       </x:c>
       <x:c r="I80" s="0" t="n">
-        <x:v>131351193.36</x:v>
+        <x:v>179834273.98</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:9">
@@ -3640,13 +3640,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G81" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="H81" s="0" t="n">
         <x:v>4413055</x:v>
       </x:c>
       <x:c r="I81" s="0" t="n">
-        <x:v>120193308.89</x:v>
+        <x:v>130992380.96</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:9">
@@ -3669,13 +3669,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G82" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="H82" s="0" t="n">
         <x:v>4848327</x:v>
       </x:c>
       <x:c r="I82" s="0" t="n">
-        <x:v>60000000</x:v>
+        <x:v>69548611.11</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:9">
@@ -3695,16 +3695,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F83" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G83" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="G83" s="0" t="n">
-        <x:v>3</x:v>
-      </x:c>
       <x:c r="H83" s="0" t="n">
-        <x:v>6078674</x:v>
+        <x:v>7078674</x:v>
       </x:c>
       <x:c r="I83" s="0" t="n">
-        <x:v>52362880</x:v>
+        <x:v>77362880</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:9">
@@ -3724,16 +3724,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F84" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G84" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="H84" s="0" t="n">
-        <x:v>3038746</x:v>
+        <x:v>5201151</x:v>
       </x:c>
       <x:c r="I84" s="0" t="n">
-        <x:v>195219913.29</x:v>
+        <x:v>248986166.98</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:9">
@@ -3753,16 +3753,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F85" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="G85" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H85" s="0" t="n">
-        <x:v>1486115</x:v>
+        <x:v>2398080</x:v>
       </x:c>
       <x:c r="I85" s="0" t="n">
-        <x:v>58476071.55</x:v>
+        <x:v>66537551.67</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:9">
@@ -3785,13 +3785,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="G86" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="H86" s="0" t="n">
         <x:v>3970214</x:v>
       </x:c>
       <x:c r="I86" s="0" t="n">
-        <x:v>61322058.15</x:v>
+        <x:v>116062382.23</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:9">
@@ -3811,16 +3811,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F87" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G87" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="H87" s="0" t="n">
-        <x:v>2943380</x:v>
+        <x:v>4828485</x:v>
       </x:c>
       <x:c r="I87" s="0" t="n">
-        <x:v>84991222.73</x:v>
+        <x:v>87794000.51</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:9">
@@ -3840,16 +3840,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F88" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G88" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H88" s="0" t="n">
-        <x:v>2212103.5</x:v>
+        <x:v>7854961.97</x:v>
       </x:c>
       <x:c r="I88" s="0" t="n">
-        <x:v>139809342.13</x:v>
+        <x:v>168854369.05</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:9">
@@ -3872,13 +3872,13 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="G89" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H89" s="0" t="n">
         <x:v>6841735.39</x:v>
       </x:c>
       <x:c r="I89" s="0" t="n">
-        <x:v>30628259.5</x:v>
+        <x:v>56043048.62</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:9">
@@ -3898,16 +3898,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F90" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="G90" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="H90" s="0" t="n">
-        <x:v>3274784.81</x:v>
+        <x:v>4274684.81</x:v>
       </x:c>
       <x:c r="I90" s="0" t="n">
-        <x:v>48748437.5</x:v>
+        <x:v>49867152.78</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:9">
@@ -3927,16 +3927,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F91" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G91" s="0" t="n">
         <x:v>13</x:v>
       </x:c>
       <x:c r="H91" s="0" t="n">
-        <x:v>6000633</x:v>
+        <x:v>8301225</x:v>
       </x:c>
       <x:c r="I91" s="0" t="n">
-        <x:v>483898524.39</x:v>
+        <x:v>485017239.67</x:v>
       </x:c>
     </x:row>
     <x:row r="92" spans="1:9">
@@ -3956,13 +3956,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F92" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G92" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="H92" s="0" t="n">
-        <x:v>3264922</x:v>
+        <x:v>4260464</x:v>
       </x:c>
       <x:c r="I92" s="0" t="n">
         <x:v>4011985</x:v>
@@ -3988,13 +3988,13 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G93" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="H93" s="0" t="n">
         <x:v>5520126.05</x:v>
       </x:c>
       <x:c r="I93" s="0" t="n">
-        <x:v>305988329.55</x:v>
+        <x:v>330322125.85</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:9">
@@ -4014,16 +4014,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F94" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G94" s="0" t="n">
         <x:v>8</x:v>
       </x:c>
       <x:c r="H94" s="0" t="n">
-        <x:v>3335293</x:v>
+        <x:v>5839230</x:v>
       </x:c>
       <x:c r="I94" s="0" t="n">
-        <x:v>53944485</x:v>
+        <x:v>54812540.56</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:9">
@@ -4049,7 +4049,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="H95" s="0" t="n">
-        <x:v>5708442</x:v>
+        <x:v>5269931</x:v>
       </x:c>
       <x:c r="I95" s="0" t="n">
         <x:v>4011985</x:v>
@@ -4075,13 +4075,13 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="G96" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="H96" s="0" t="n">
         <x:v>5293624</x:v>
       </x:c>
       <x:c r="I96" s="0" t="n">
-        <x:v>124385125.65</x:v>
+        <x:v>147563142.82</x:v>
       </x:c>
     </x:row>
     <x:row r="97" spans="1:9">
@@ -4104,13 +4104,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="G97" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H97" s="0" t="n">
         <x:v>3093796</x:v>
       </x:c>
       <x:c r="I97" s="0" t="n">
-        <x:v>29338620</x:v>
+        <x:v>36860100.12</x:v>
       </x:c>
     </x:row>
     <x:row r="98" spans="1:9">
@@ -4133,13 +4133,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G98" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H98" s="0" t="n">
         <x:v>5523863</x:v>
       </x:c>
       <x:c r="I98" s="0" t="n">
-        <x:v>112106553.74</x:v>
+        <x:v>148264783.74</x:v>
       </x:c>
     </x:row>
     <x:row r="99" spans="1:9">
@@ -4191,13 +4191,13 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="G100" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H100" s="0" t="n">
         <x:v>4802833.39</x:v>
       </x:c>
       <x:c r="I100" s="0" t="n">
-        <x:v>125222216.38</x:v>
+        <x:v>155963966.16</x:v>
       </x:c>
     </x:row>
     <x:row r="101" spans="1:9">
@@ -4220,13 +4220,13 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="G101" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H101" s="0" t="n">
         <x:v>4863510.15</x:v>
       </x:c>
       <x:c r="I101" s="0" t="n">
-        <x:v>196945307.54</x:v>
+        <x:v>255539944.72</x:v>
       </x:c>
     </x:row>
     <x:row r="102" spans="1:9">
@@ -4249,13 +4249,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="G102" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="H102" s="0" t="n">
         <x:v>1339759</x:v>
       </x:c>
       <x:c r="I102" s="0" t="n">
-        <x:v>9480634.8</x:v>
+        <x:v>17002114.92</x:v>
       </x:c>
     </x:row>
     <x:row r="103" spans="1:9">
@@ -4275,16 +4275,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F103" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G103" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="H103" s="0" t="n">
-        <x:v>4462686</x:v>
+        <x:v>5439921</x:v>
       </x:c>
       <x:c r="I103" s="0" t="n">
-        <x:v>61508589.16</x:v>
+        <x:v>63874989.63</x:v>
       </x:c>
     </x:row>
     <x:row r="104" spans="1:9">
@@ -4304,13 +4304,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F104" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G104" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H104" s="0" t="n">
-        <x:v>5232600.4</x:v>
+        <x:v>5614860.4</x:v>
       </x:c>
     </x:row>
     <x:row r="105" spans="1:9">
@@ -4330,16 +4330,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F105" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="G105" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="H105" s="0" t="n">
-        <x:v>5687820</x:v>
+        <x:v>6136870.44</x:v>
       </x:c>
       <x:c r="I105" s="0" t="n">
-        <x:v>304227118</x:v>
+        <x:v>331727118</x:v>
       </x:c>
     </x:row>
     <x:row r="106" spans="1:9">
@@ -4359,16 +4359,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F106" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G106" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H106" s="0" t="n">
-        <x:v>4314293</x:v>
+        <x:v>5314293</x:v>
       </x:c>
       <x:c r="I106" s="0" t="n">
-        <x:v>12416405.55</x:v>
+        <x:v>19937885.67</x:v>
       </x:c>
     </x:row>
     <x:row r="107" spans="1:9">
@@ -4397,7 +4397,7 @@
         <x:v>7531023.62</x:v>
       </x:c>
       <x:c r="I107" s="0" t="n">
-        <x:v>128799251.9</x:v>
+        <x:v>129341590.79</x:v>
       </x:c>
     </x:row>
     <x:row r="108" spans="1:9">
@@ -4420,13 +4420,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G108" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H108" s="0" t="n">
         <x:v>4291757</x:v>
       </x:c>
       <x:c r="I108" s="0" t="n">
-        <x:v>14428620</x:v>
+        <x:v>89863856.12</x:v>
       </x:c>
     </x:row>
     <x:row r="109" spans="1:9">
@@ -4446,16 +4446,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F109" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G109" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H109" s="0" t="n">
-        <x:v>3669914</x:v>
+        <x:v>7213513</x:v>
       </x:c>
       <x:c r="I109" s="0" t="n">
-        <x:v>146376970.61</x:v>
+        <x:v>196376970.61</x:v>
       </x:c>
     </x:row>
     <x:row r="110" spans="1:9">
@@ -4478,13 +4478,13 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="G110" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="H110" s="0" t="n">
-        <x:v>5805625.28</x:v>
+        <x:v>6663120.28</x:v>
       </x:c>
       <x:c r="I110" s="0" t="n">
-        <x:v>153294451.57</x:v>
+        <x:v>263918743.72</x:v>
       </x:c>
     </x:row>
     <x:row r="111" spans="1:9">
@@ -4507,13 +4507,13 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="G111" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="H111" s="0" t="n">
         <x:v>2662942</x:v>
       </x:c>
       <x:c r="I111" s="0" t="n">
-        <x:v>158576410.16</x:v>
+        <x:v>184345299.05</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="1:9">
@@ -4579,16 +4579,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F114" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G114" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="H114" s="0" t="n">
-        <x:v>5753838</x:v>
+        <x:v>6929846</x:v>
       </x:c>
       <x:c r="I114" s="0" t="n">
-        <x:v>242340014.65</x:v>
+        <x:v>281053784.75</x:v>
       </x:c>
     </x:row>
     <x:row r="115" spans="1:9">
@@ -4608,13 +4608,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F115" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="G115" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="H115" s="0" t="n">
-        <x:v>5332269.31</x:v>
+        <x:v>8330634.31</x:v>
       </x:c>
       <x:c r="I115" s="0" t="n">
         <x:v>16000000</x:v>
@@ -4640,13 +4640,13 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="G116" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="H116" s="0" t="n">
-        <x:v>8077288.56</x:v>
+        <x:v>9215878.56</x:v>
       </x:c>
       <x:c r="I116" s="0" t="n">
-        <x:v>16000000</x:v>
+        <x:v>30750000</x:v>
       </x:c>
     </x:row>
     <x:row r="117" spans="1:9">
@@ -4672,7 +4672,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="H117" s="0" t="n">
-        <x:v>4853879.67</x:v>
+        <x:v>6853879.67</x:v>
       </x:c>
       <x:c r="I117" s="0" t="n">
         <x:v>16000000</x:v>
@@ -4698,13 +4698,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="G118" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H118" s="0" t="n">
         <x:v>1034409</x:v>
       </x:c>
       <x:c r="I118" s="0" t="n">
-        <x:v>60146620</x:v>
+        <x:v>67668100.12</x:v>
       </x:c>
     </x:row>
     <x:row r="119" spans="1:9">
@@ -4744,7 +4744,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E120" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="F120" s="0" t="n">
         <x:v>5</x:v>
@@ -4799,16 +4799,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F122" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="G122" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="H122" s="0" t="n">
-        <x:v>6116312.27</x:v>
+        <x:v>7116312.27</x:v>
       </x:c>
       <x:c r="I122" s="0" t="n">
-        <x:v>199465762.63</x:v>
+        <x:v>304896257.39</x:v>
       </x:c>
     </x:row>
     <x:row r="123" spans="1:9">
@@ -4828,16 +4828,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F123" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G123" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H123" s="0" t="n">
-        <x:v>3282807</x:v>
+        <x:v>4182807</x:v>
       </x:c>
       <x:c r="I123" s="0" t="n">
-        <x:v>92432637.5</x:v>
+        <x:v>118551352.78</x:v>
       </x:c>
     </x:row>
     <x:row r="124" spans="1:9">
@@ -4886,16 +4886,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F125" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G125" s="0" t="n">
         <x:v>8</x:v>
       </x:c>
       <x:c r="H125" s="0" t="n">
-        <x:v>2623304</x:v>
+        <x:v>4958625</x:v>
       </x:c>
       <x:c r="I125" s="0" t="n">
-        <x:v>74969639.65</x:v>
+        <x:v>72183409.75</x:v>
       </x:c>
     </x:row>
     <x:row r="126" spans="1:9">
@@ -4938,16 +4938,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F127" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="G127" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H127" s="0" t="n">
-        <x:v>2100732</x:v>
+        <x:v>3056753</x:v>
       </x:c>
       <x:c r="I127" s="0" t="n">
-        <x:v>110965114</x:v>
+        <x:v>118486594.12</x:v>
       </x:c>
     </x:row>
     <x:row r="128" spans="1:9">
@@ -4970,13 +4970,13 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="G128" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H128" s="0" t="n">
         <x:v>4628638</x:v>
       </x:c>
       <x:c r="I128" s="0" t="n">
-        <x:v>158099868</x:v>
+        <x:v>170067980.47</x:v>
       </x:c>
     </x:row>
     <x:row r="129" spans="1:9">
@@ -4999,13 +4999,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="G129" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="H129" s="0" t="n">
         <x:v>1721820.11</x:v>
       </x:c>
       <x:c r="I129" s="0" t="n">
-        <x:v>414610485</x:v>
+        <x:v>459654941.79</x:v>
       </x:c>
     </x:row>
     <x:row r="130" spans="1:9">
@@ -5028,13 +5028,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="G130" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H130" s="0" t="n">
         <x:v>600176</x:v>
       </x:c>
       <x:c r="I130" s="0" t="n">
-        <x:v>30200000</x:v>
+        <x:v>88462704.83</x:v>
       </x:c>
     </x:row>
     <x:row r="131" spans="1:9">
@@ -5054,16 +5054,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F131" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G131" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
       <x:c r="H131" s="0" t="n">
-        <x:v>6489399</x:v>
+        <x:v>7467632</x:v>
       </x:c>
       <x:c r="I131" s="0" t="n">
-        <x:v>105693354.16</x:v>
+        <x:v>106072115.74</x:v>
       </x:c>
     </x:row>
     <x:row r="132" spans="1:9">
@@ -5083,16 +5083,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F132" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G132" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="H132" s="0" t="n">
-        <x:v>4601268.4</x:v>
+        <x:v>5486368.4</x:v>
       </x:c>
       <x:c r="I132" s="0" t="n">
-        <x:v>24697689.58</x:v>
+        <x:v>27441877.31</x:v>
       </x:c>
     </x:row>
     <x:row r="133" spans="1:9">
@@ -5121,7 +5121,7 @@
         <x:v>3275952</x:v>
       </x:c>
       <x:c r="I133" s="0" t="n">
-        <x:v>43986715.71</x:v>
+        <x:v>44916338.12</x:v>
       </x:c>
     </x:row>
     <x:row r="134" spans="1:9">
@@ -5144,13 +5144,13 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="G134" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="H134" s="0" t="n">
         <x:v>4385426.85</x:v>
       </x:c>
       <x:c r="I134" s="0" t="n">
-        <x:v>28637594.8</x:v>
+        <x:v>52629818.08</x:v>
       </x:c>
     </x:row>
     <x:row r="135" spans="1:9">
@@ -5196,16 +5196,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F136" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G136" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="H136" s="0" t="n">
-        <x:v>5052267</x:v>
+        <x:v>5699687</x:v>
       </x:c>
       <x:c r="I136" s="0" t="n">
-        <x:v>145969586</x:v>
+        <x:v>173469586</x:v>
       </x:c>
     </x:row>
     <x:row r="137" spans="1:9">
@@ -5228,13 +5228,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="G137" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H137" s="0" t="n">
         <x:v>4334250</x:v>
       </x:c>
       <x:c r="I137" s="0" t="n">
-        <x:v>280395519.67</x:v>
+        <x:v>343613110.26</x:v>
       </x:c>
     </x:row>
     <x:row r="138" spans="1:9">
@@ -5254,16 +5254,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F138" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G138" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H138" s="0" t="n">
-        <x:v>6771017</x:v>
+        <x:v>7469000</x:v>
       </x:c>
       <x:c r="I138" s="0" t="n">
-        <x:v>57298444.79</x:v>
+        <x:v>73956771.99</x:v>
       </x:c>
     </x:row>
     <x:row r="139" spans="1:9">
@@ -5312,16 +5312,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F140" s="0" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G140" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="G140" s="0" t="n">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="H140" s="0" t="n">
-        <x:v>6278288.39</x:v>
+        <x:v>6895251.39</x:v>
       </x:c>
       <x:c r="I140" s="0" t="n">
-        <x:v>91913901.21</x:v>
+        <x:v>118453536.7</x:v>
       </x:c>
     </x:row>
     <x:row r="141" spans="1:9">
@@ -5344,13 +5344,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="G141" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H141" s="0" t="n">
         <x:v>6110929.9</x:v>
       </x:c>
       <x:c r="I141" s="0" t="n">
-        <x:v>54985029</x:v>
+        <x:v>78070535.46</x:v>
       </x:c>
     </x:row>
     <x:row r="142" spans="1:9">
@@ -5370,16 +5370,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F142" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="G142" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="H142" s="0" t="n">
-        <x:v>5600554.99</x:v>
+        <x:v>7100554.99</x:v>
       </x:c>
       <x:c r="I142" s="0" t="n">
-        <x:v>34814854.28</x:v>
+        <x:v>46873578.28</x:v>
       </x:c>
     </x:row>
     <x:row r="143" spans="1:9">
@@ -5399,16 +5399,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F143" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="G143" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
       <x:c r="H143" s="0" t="n">
-        <x:v>4825957</x:v>
+        <x:v>5608729</x:v>
       </x:c>
       <x:c r="I143" s="0" t="n">
-        <x:v>239715078.73</x:v>
+        <x:v>246379511.6</x:v>
       </x:c>
     </x:row>
     <x:row r="144" spans="1:9">
@@ -5431,10 +5431,13 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="G144" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="H144" s="0" t="n">
         <x:v>3046858</x:v>
+      </x:c>
+      <x:c r="I144" s="0" t="n">
+        <x:v>27500000</x:v>
       </x:c>
     </x:row>
     <x:row r="145" spans="1:9">
@@ -5457,13 +5460,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="G145" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H145" s="0" t="n">
         <x:v>6144806</x:v>
       </x:c>
       <x:c r="I145" s="0" t="n">
-        <x:v>45490634.8</x:v>
+        <x:v>53012114.92</x:v>
       </x:c>
     </x:row>
     <x:row r="146" spans="1:9">
@@ -5486,13 +5489,13 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="G146" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="H146" s="0" t="n">
         <x:v>4638344</x:v>
       </x:c>
       <x:c r="I146" s="0" t="n">
-        <x:v>105851672.89</x:v>
+        <x:v>220095074.42</x:v>
       </x:c>
     </x:row>
     <x:row r="147" spans="1:9">
@@ -5535,13 +5538,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F148" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="G148" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
       <x:c r="H148" s="0" t="n">
-        <x:v>7863888.89</x:v>
+        <x:v>7628175.89</x:v>
       </x:c>
       <x:c r="I148" s="0" t="n">
         <x:v>69550975.77</x:v>
@@ -5567,13 +5570,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="G149" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="H149" s="0" t="n">
         <x:v>2225319</x:v>
       </x:c>
       <x:c r="I149" s="0" t="n">
-        <x:v>159726600.74</x:v>
+        <x:v>189726600.74</x:v>
       </x:c>
     </x:row>
     <x:row r="150" spans="1:9">
@@ -5596,13 +5599,13 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G150" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H150" s="0" t="n">
         <x:v>6718814</x:v>
       </x:c>
       <x:c r="I150" s="0" t="n">
-        <x:v>96460911</x:v>
+        <x:v>105962391.12</x:v>
       </x:c>
     </x:row>
     <x:row r="151" spans="1:9">
@@ -5677,13 +5680,13 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="F153" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G153" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H153" s="0" t="n">
-        <x:v>3486360</x:v>
+        <x:v>6386348</x:v>
       </x:c>
     </x:row>
     <x:row r="154" spans="1:9">
@@ -5706,13 +5709,13 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="G154" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H154" s="0" t="n">
-        <x:v>4538878.79</x:v>
+        <x:v>5001577</x:v>
       </x:c>
       <x:c r="I154" s="0" t="n">
-        <x:v>138727811.19</x:v>
+        <x:v>146763290.21</x:v>
       </x:c>
     </x:row>
     <x:row r="155" spans="1:9">
@@ -5732,16 +5735,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F155" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G155" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H155" s="0" t="n">
-        <x:v>4164077</x:v>
+        <x:v>5017647</x:v>
       </x:c>
       <x:c r="I155" s="0" t="n">
-        <x:v>35432883</x:v>
+        <x:v>60432883</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>